<commit_message>
Added Import For Church/District/DistrictState/Section/
</commit_message>
<xml_diff>
--- a/src/SFA/wwwroot/resources/sections/Section.xlsx
+++ b/src/SFA/wwwroot/resources/sections/Section.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEANR\OneDrive\Documents\GitHub\gmdeputation\src\SFA\wwwroot\resources\sections\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741541D8-E579-4CC1-A860-5EED2BE97D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="37425" yWindow="3510" windowWidth="22785" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,30 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>District Code</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>Section Name</t>
-  </si>
-  <si>
-    <t>D001</t>
-  </si>
-  <si>
-    <t>Saltlake</t>
-  </si>
-  <si>
-    <t>Esplanade</t>
-  </si>
-  <si>
-    <t>Park Street</t>
+    <t>District ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,20 +347,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,30 +368,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>